<commit_message>
design and power information
</commit_message>
<xml_diff>
--- a/design.xlsx
+++ b/design.xlsx
@@ -8,24 +8,37 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/74db7c87a9029f2a/Documents/PCB/SmallFlight1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="250" documentId="11_F25DC773A252ABDACC1048E409DB493A5ADE58E8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0BFFAFA4-9184-48D7-80F7-95634DCC6AD0}"/>
+  <xr:revisionPtr revIDLastSave="364" documentId="11_F25DC773A252ABDACC1048E409DB493A5ADE58E8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{63C0DE87-38A7-4B5C-B76B-07491D3C1D10}"/>
   <bookViews>
-    <workbookView xWindow="8145" yWindow="0" windowWidth="18945" windowHeight="15585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11865" yWindow="2055" windowWidth="16155" windowHeight="10935" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Design" sheetId="1" r:id="rId1"/>
+    <sheet name="Ideation" sheetId="1" r:id="rId1"/>
+    <sheet name="Parts" sheetId="3" r:id="rId2"/>
+    <sheet name="Power" sheetId="2" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="73">
   <si>
     <t xml:space="preserve">Estimated Flight Profile </t>
   </si>
@@ -93,9 +106,6 @@
     <t>Component Requirements</t>
   </si>
   <si>
-    <t>Supporting Requirements 1</t>
-  </si>
-  <si>
     <t>Supporting capacitors and resistors, Serial communication line</t>
   </si>
   <si>
@@ -225,19 +235,28 @@
     <t>https://core-electronics.com.au/micro-sd-card-module-3-3-and-5v-compatible.html</t>
   </si>
   <si>
-    <t>Core Part Selection</t>
-  </si>
-  <si>
-    <t>Core Power Requirements</t>
-  </si>
-  <si>
-    <t>Voltage</t>
-  </si>
-  <si>
-    <t>Current</t>
-  </si>
-  <si>
-    <t>Power Circuitry Selection</t>
+    <t>Min</t>
+  </si>
+  <si>
+    <t>Max</t>
+  </si>
+  <si>
+    <t>Voltage (V)</t>
+  </si>
+  <si>
+    <t>Current (mA)</t>
+  </si>
+  <si>
+    <t>Typical</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Supporting Requirements </t>
+  </si>
+  <si>
+    <t>Power Requirements</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Part Selection</t>
   </si>
 </sst>
 </file>
@@ -285,7 +304,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -308,49 +327,12 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -364,19 +346,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -660,10 +636,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I35"/>
+  <dimension ref="A1:H7"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -677,54 +653,54 @@
     <col min="10" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
+    <row r="1" spans="1:8" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
-      <c r="E1" s="5" t="s">
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+      <c r="E1" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5"/>
-      <c r="H1" s="5"/>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="5"/>
-      <c r="B2" s="5"/>
-      <c r="C2" s="5"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
+      <c r="H1" s="6"/>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="6"/>
+      <c r="B2" s="6"/>
+      <c r="C2" s="6"/>
       <c r="E2" s="3" t="s">
         <v>8</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G2" s="3" t="s">
         <v>21</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="5"/>
-      <c r="B3" s="5"/>
-      <c r="C3" s="5"/>
+        <v>70</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="6"/>
+      <c r="B3" s="6"/>
+      <c r="C3" s="6"/>
       <c r="E3" s="2" t="s">
         <v>9</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>13</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>1</v>
       </c>
@@ -738,16 +714,16 @@
         <v>10</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G4" s="2" t="s">
         <v>14</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>2</v>
       </c>
@@ -761,18 +737,18 @@
         <v>11</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G5" s="2" t="s">
         <v>16</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B6" s="2">
         <v>116</v>
@@ -784,16 +760,16 @@
         <v>12</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G6" s="2" t="s">
         <v>15</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>3</v>
       </c>
@@ -807,259 +783,427 @@
         <v>18</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G7" s="2" t="s">
         <v>17</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E10" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="F10" s="5"/>
-      <c r="G10" s="5"/>
-      <c r="H10" s="5"/>
-      <c r="I10" s="5"/>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="E11" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="F11" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="G11" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="H11" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="I11" s="3" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="E12" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="F12" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="G12" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="H12" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="I12" s="2" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="E13" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="F13" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="G13" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="H13" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="I13" s="2" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="E14" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="F14" s="2">
-        <v>1040310811</v>
-      </c>
-      <c r="G14" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="H14" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="I14" s="2" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="E15" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="F15" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="G15" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="H15" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="I15" s="2" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="E16" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="F16" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="G16" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="H16" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="I16" s="2" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="17" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="E17" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="F17" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="G17" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="H17" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="I17" s="9" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="18" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="E18" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="F18" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="G18" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="H18" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="I18" s="2" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="21" spans="5:9" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E21" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="F21" s="7"/>
-      <c r="G21" s="8"/>
-    </row>
-    <row r="22" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="E22" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="F22" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="G22" s="3" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="23" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="E23" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="F23" s="2"/>
-      <c r="G23" s="2"/>
-    </row>
-    <row r="24" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="E24" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="F24" s="2"/>
-      <c r="G24" s="2"/>
-    </row>
-    <row r="25" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="E25" s="2">
-        <v>1040310811</v>
-      </c>
-      <c r="F25" s="2"/>
-      <c r="G25" s="2"/>
-    </row>
-    <row r="26" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="E26" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="F26" s="2"/>
-      <c r="G26" s="2"/>
-    </row>
-    <row r="27" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="E27" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="F27" s="2"/>
-      <c r="G27" s="2"/>
-    </row>
-    <row r="28" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="E28" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="F28" s="2"/>
-      <c r="G28" s="2"/>
-    </row>
-    <row r="29" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="E29" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="F29" s="2"/>
-      <c r="G29" s="2"/>
-    </row>
-    <row r="32" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="E32" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="F32" s="2"/>
-      <c r="G32" s="2"/>
-    </row>
-    <row r="33" spans="5:7" x14ac:dyDescent="0.25">
-      <c r="E33" s="2"/>
-      <c r="F33" s="2"/>
-      <c r="G33" s="2"/>
-    </row>
-    <row r="34" spans="5:7" x14ac:dyDescent="0.25">
-      <c r="E34" s="2"/>
-      <c r="F34" s="2"/>
-      <c r="G34" s="2"/>
-    </row>
-    <row r="35" spans="5:7" x14ac:dyDescent="0.25">
-      <c r="E35" s="2"/>
-      <c r="F35" s="2"/>
-      <c r="G35" s="2"/>
+        <v>24</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="2">
     <mergeCell ref="E1:H1"/>
     <mergeCell ref="A1:C3"/>
-    <mergeCell ref="E10:I10"/>
-    <mergeCell ref="E21:G21"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B80A695A-9DE3-4995-ACC8-7BE4B53153AB}">
+  <dimension ref="A1:E9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:E9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="30.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="45.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.7109375" customWidth="1"/>
+    <col min="5" max="5" width="106.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B5" s="2">
+        <v>1040310811</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:E1"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="I17" r:id="rId1" xr:uid="{D732040F-E26F-4767-961E-9316FE395C70}"/>
+    <hyperlink ref="E8" r:id="rId1" xr:uid="{29E36415-BC89-409B-9AAB-729EDB483B27}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1B774BC-19AE-4085-853D-BC5D7AB716CB}">
+  <dimension ref="A1:G10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="45.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="F2" s="7"/>
+      <c r="G2" s="7"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="7"/>
+      <c r="B3" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B4" s="2">
+        <v>1.7</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4" s="2">
+        <v>3.6</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G4" s="2">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B5" s="2">
+        <v>2.7</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D5" s="2">
+        <v>3.6</v>
+      </c>
+      <c r="E5" s="2">
+        <v>1E-3</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G5" s="2">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="2">
+        <v>1040310811</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D6" s="2">
+        <v>10</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="B7" s="2">
+        <v>1.71</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D7" s="2">
+        <v>3.6</v>
+      </c>
+      <c r="E7" s="2">
+        <v>1E-4</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G7" s="2">
+        <v>3.5999999999999999E-3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B8" s="2">
+        <v>1.71</v>
+      </c>
+      <c r="C8" s="2">
+        <v>1.8</v>
+      </c>
+      <c r="D8" s="2">
+        <v>3.6</v>
+      </c>
+      <c r="E8" s="2">
+        <v>9.4999999999999998E-3</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G8" s="2">
+        <v>0.55000000000000004</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B9" s="2">
+        <v>4.8</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D9" s="2">
+        <v>6</v>
+      </c>
+      <c r="E9" s="2">
+        <v>200</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G9" s="2">
+        <v>1130</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B10" s="2">
+        <v>1.62</v>
+      </c>
+      <c r="C10" s="2">
+        <v>1.8</v>
+      </c>
+      <c r="D10" s="2">
+        <v>3.6</v>
+      </c>
+      <c r="E10" s="2">
+        <v>0.75</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G10" s="2">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="B2:D2"/>
+    <mergeCell ref="E2:G2"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="A1:G1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>